<commit_message>
2017.5.15 beta for SAM for India updates
</commit_message>
<xml_diff>
--- a/deploy/runtime/spreadsheets/PV_for_India.xlsx
+++ b/deploy/runtime/spreadsheets/PV_for_India.xlsx
@@ -1,17 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17329"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17927"/>
   <workbookPr filterPrivacy="1" showInkAnnotation="0" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="10788" yWindow="-24" windowWidth="10836" windowHeight="10740" tabRatio="930" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28450" windowHeight="11610" tabRatio="930" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="General Notes" sheetId="19" r:id="rId1"/>
-    <sheet name="Assumptions" sheetId="12" r:id="rId2"/>
-    <sheet name="Calculations" sheetId="13" r:id="rId3"/>
-    <sheet name="Term Loan" sheetId="14" r:id="rId4"/>
-    <sheet name="Working Capital" sheetId="15" r:id="rId5"/>
+    <sheet name="Results Summary" sheetId="20" r:id="rId2"/>
+    <sheet name="Assumptions" sheetId="12" r:id="rId3"/>
+    <sheet name="Calculations" sheetId="13" r:id="rId4"/>
+    <sheet name="Term Loan" sheetId="14" r:id="rId5"/>
+    <sheet name="Working Capital" sheetId="15" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="analysis_period">Assumptions!$F$8</definedName>
@@ -112,6 +113,7 @@
     <definedName name="depr_itc_sta_sl_39">#REF!</definedName>
     <definedName name="depr_itc_sta_sl_5">#REF!</definedName>
     <definedName name="dscr_reserve_months">#REF!</definedName>
+    <definedName name="dscr_summary">'Results Summary'!$D$8</definedName>
     <definedName name="equip_reserve_depr_fed">#REF!</definedName>
     <definedName name="equip_reserve_depr_sta">#REF!</definedName>
     <definedName name="equip1_reserve_cost">#REF!</definedName>
@@ -171,6 +173,8 @@
     <definedName name="inflation_rate">#REF!</definedName>
     <definedName name="installed_capacity">Assumptions!$F$5</definedName>
     <definedName name="insurance_rate">#REF!</definedName>
+    <definedName name="irr_summary">'Results Summary'!$D$6</definedName>
+    <definedName name="irr_year_summary">'Results Summary'!$D$7</definedName>
     <definedName name="IRRTarget">#REF!</definedName>
     <definedName name="IRRTargetYear">#REF!</definedName>
     <definedName name="itc_fed_amount">#REF!</definedName>
@@ -187,6 +191,7 @@
     <definedName name="itc_sta_percent_deprbas_fed">#REF!</definedName>
     <definedName name="itc_sta_percent_deprbas_sta">#REF!</definedName>
     <definedName name="itc_sta_percent_maxvalue">#REF!</definedName>
+    <definedName name="lcog_summary">'Results Summary'!$D$4</definedName>
     <definedName name="loan_moratorium">Assumptions!$F$16</definedName>
     <definedName name="loan_principal">Assumptions!$F$15</definedName>
     <definedName name="months_receivables_reserve">Assumptions!$F$31</definedName>
@@ -194,6 +199,7 @@
     <definedName name="MortgageSizeOfDebt">#REF!</definedName>
     <definedName name="nominal_discount_rate">Assumptions!$F$23</definedName>
     <definedName name="NominalDiscountRate">#REF!</definedName>
+    <definedName name="npv_summary">'Results Summary'!$D$5</definedName>
     <definedName name="om_acceleration">Assumptions!$F$34</definedName>
     <definedName name="om_capacity">#REF!</definedName>
     <definedName name="om_capacity_escal">#REF!</definedName>
@@ -266,7 +272,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="86">
   <si>
     <t>%</t>
   </si>
@@ -503,13 +509,38 @@
   </si>
   <si>
     <t>Interest Payment</t>
+  </si>
+  <si>
+    <t>Year IRR is Achieved</t>
+  </si>
+  <si>
+    <t>Net Present Value (NPV)</t>
+  </si>
+  <si>
+    <t>Internal Rate of Return (IRR)</t>
+  </si>
+  <si>
+    <t>Levellized Cost of Electricity Generation (LCOE)</t>
+  </si>
+  <si>
+    <t>Minimum Debt Service Coverage Ratio (DSCR)</t>
+  </si>
+  <si>
+    <t>Output</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rs </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -534,6 +565,13 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -605,12 +643,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -635,6 +674,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -642,7 +684,8 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
+    <cellStyle name="Comma" xfId="3" builtinId="3"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
@@ -1124,7 +1167,7 @@
       <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1136,392 +1179,67 @@
   <sheetPr>
     <tabColor theme="6" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="D3:H35"/>
+  <dimension ref="B3:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.77734375" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.44140625" customWidth="1"/>
-    <col min="7" max="7" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.81640625" customWidth="1"/>
+    <col min="4" max="4" width="12.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D3" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" s="10" t="s">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B3" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="C3" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="D3" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-    </row>
-    <row r="4" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D4" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="E4" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="16">
-        <v>1665953</v>
-      </c>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-    </row>
-    <row r="5" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D5" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="F5" s="11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D6" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="F6" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D7" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="E7" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="F7" s="11">
-        <v>0.19</v>
-      </c>
-    </row>
-    <row r="8" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D8" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="E8" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="F8" s="11">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D9" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="E9" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="F9" s="11">
-        <v>530.02</v>
-      </c>
-    </row>
-    <row r="10" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D10" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="F10" s="11">
-        <f>analysis_period</f>
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D11" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="E11" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="F11" s="11">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="12" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D12" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="E12" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="F12" s="11">
-        <f>100-F11</f>
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D13" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="E13" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="F13" s="11">
-        <f>F11/100*F9</f>
-        <v>371.01399999999995</v>
-      </c>
-    </row>
-    <row r="14" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D14" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="E14" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="F14" s="11">
-        <f>F12/100*F9</f>
-        <v>159.006</v>
-      </c>
-    </row>
-    <row r="15" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D15" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="E15" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="F15" s="11">
-        <f>F13</f>
-        <v>371.01399999999995</v>
-      </c>
-    </row>
-    <row r="16" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D16" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="E16" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="F16" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D17" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="E17" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="F17" s="11">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D18" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="E18" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="F18" s="11">
-        <v>12.76</v>
-      </c>
-    </row>
-    <row r="19" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D19" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="E19" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="F19" s="11">
-        <f>F14+'Working Capital'!C7</f>
-        <v>175.38812095</v>
-      </c>
-    </row>
-    <row r="20" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D20" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="E20" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="F20" s="11">
-        <f>F19-'Working Capital'!C7</f>
-        <v>159.006</v>
-      </c>
-    </row>
-    <row r="21" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D21" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="E21" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="F21" s="11">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D22" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="E22" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="F22" s="11">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="23" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D23" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="E23" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="F23" s="12">
-        <v>10.7</v>
-      </c>
-    </row>
-    <row r="24" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D24" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="E24" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="F24" s="12">
-        <v>33.99</v>
-      </c>
-    </row>
-    <row r="25" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D25" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="E25" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="F25" s="12">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="26" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D26" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="E26" s="11"/>
-      <c r="F26" s="13" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D27" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="E27" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="F27" s="11">
-        <v>5.83</v>
-      </c>
-    </row>
-    <row r="28" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D28" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="E28" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="F28" s="11">
-        <v>1.54</v>
-      </c>
-    </row>
-    <row r="29" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D29" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="E29" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="F29" s="11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D30" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="E30" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="F30" s="11">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="31" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D31" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="E31" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="F31" s="11">
-        <v>2.1</v>
-      </c>
-    </row>
-    <row r="32" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D32" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="E32" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="F32" s="11">
-        <v>13.26</v>
-      </c>
-    </row>
-    <row r="33" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D33" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="E33" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="F33" s="11">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="34" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D34" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="E34" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="F34" s="14">
-        <v>5.72</v>
-      </c>
-    </row>
-    <row r="35" spans="4:6" x14ac:dyDescent="0.3">
-      <c r="D35" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="E35" s="15" t="s">
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C4" t="s">
         <v>52</v>
       </c>
-      <c r="F35" s="15">
-        <v>5.69</v>
-      </c>
+      <c r="D4" s="23"/>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
+        <v>80</v>
+      </c>
+      <c r="C5" t="s">
+        <v>85</v>
+      </c>
+      <c r="D5" s="24"/>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="23"/>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B7" t="s">
+        <v>79</v>
+      </c>
+      <c r="D7" s="24"/>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B8" t="s">
+        <v>83</v>
+      </c>
+      <c r="D8" s="23"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1534,21 +1252,419 @@
   <sheetPr>
     <tabColor theme="6" tint="0.39997558519241921"/>
   </sheetPr>
+  <dimension ref="D3:H35"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.81640625" customWidth="1"/>
+    <col min="5" max="5" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.453125" customWidth="1"/>
+    <col min="7" max="7" width="26.36328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="4:8" x14ac:dyDescent="0.35">
+      <c r="D3" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+    </row>
+    <row r="4" spans="4:8" x14ac:dyDescent="0.35">
+      <c r="D4" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="16">
+        <v>1665953</v>
+      </c>
+      <c r="G4" s="9"/>
+      <c r="H4" s="9"/>
+    </row>
+    <row r="5" spans="4:8" x14ac:dyDescent="0.35">
+      <c r="D5" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="4:8" x14ac:dyDescent="0.35">
+      <c r="D6" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="F6" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="4:8" x14ac:dyDescent="0.35">
+      <c r="D7" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="F7" s="11">
+        <v>0.19</v>
+      </c>
+    </row>
+    <row r="8" spans="4:8" x14ac:dyDescent="0.35">
+      <c r="D8" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" s="11">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="4:8" x14ac:dyDescent="0.35">
+      <c r="D9" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" s="11">
+        <v>530.02</v>
+      </c>
+    </row>
+    <row r="10" spans="4:8" x14ac:dyDescent="0.35">
+      <c r="D10" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" s="11">
+        <f>analysis_period</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="4:8" x14ac:dyDescent="0.35">
+      <c r="D11" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="F11" s="11">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="4:8" x14ac:dyDescent="0.35">
+      <c r="D12" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="F12" s="11">
+        <f>100-F11</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="4:8" x14ac:dyDescent="0.35">
+      <c r="D13" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="F13" s="11">
+        <f>F11/100*F9</f>
+        <v>371.01399999999995</v>
+      </c>
+    </row>
+    <row r="14" spans="4:8" x14ac:dyDescent="0.35">
+      <c r="D14" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="F14" s="11">
+        <f>F12/100*F9</f>
+        <v>159.006</v>
+      </c>
+    </row>
+    <row r="15" spans="4:8" x14ac:dyDescent="0.35">
+      <c r="D15" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="F15" s="11">
+        <f>F13</f>
+        <v>371.01399999999995</v>
+      </c>
+    </row>
+    <row r="16" spans="4:8" x14ac:dyDescent="0.35">
+      <c r="D16" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="F16" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="4:6" x14ac:dyDescent="0.35">
+      <c r="D17" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E17" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="F17" s="11">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="4:6" x14ac:dyDescent="0.35">
+      <c r="D18" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="E18" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="F18" s="11">
+        <v>12.76</v>
+      </c>
+    </row>
+    <row r="19" spans="4:6" x14ac:dyDescent="0.35">
+      <c r="D19" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="F19" s="11">
+        <f>F14+'Working Capital'!C7</f>
+        <v>175.38812095</v>
+      </c>
+    </row>
+    <row r="20" spans="4:6" x14ac:dyDescent="0.35">
+      <c r="D20" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="F20" s="11">
+        <f>F19-'Working Capital'!C7</f>
+        <v>159.006</v>
+      </c>
+    </row>
+    <row r="21" spans="4:6" x14ac:dyDescent="0.35">
+      <c r="D21" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="F21" s="11">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="4:6" x14ac:dyDescent="0.35">
+      <c r="D22" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="E22" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="F22" s="11">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="4:6" x14ac:dyDescent="0.35">
+      <c r="D23" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="F23" s="12">
+        <v>10.7</v>
+      </c>
+    </row>
+    <row r="24" spans="4:6" x14ac:dyDescent="0.35">
+      <c r="D24" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="E24" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="F24" s="12">
+        <v>33.99</v>
+      </c>
+    </row>
+    <row r="25" spans="4:6" x14ac:dyDescent="0.35">
+      <c r="D25" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="E25" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="F25" s="12">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="4:6" x14ac:dyDescent="0.35">
+      <c r="D26" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="E26" s="11"/>
+      <c r="F26" s="13" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="4:6" x14ac:dyDescent="0.35">
+      <c r="D27" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="E27" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="F27" s="11">
+        <v>5.83</v>
+      </c>
+    </row>
+    <row r="28" spans="4:6" x14ac:dyDescent="0.35">
+      <c r="D28" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="E28" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="F28" s="11">
+        <v>1.54</v>
+      </c>
+    </row>
+    <row r="29" spans="4:6" x14ac:dyDescent="0.35">
+      <c r="D29" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E29" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="F29" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="4:6" x14ac:dyDescent="0.35">
+      <c r="D30" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E30" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="F30" s="11">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="4:6" x14ac:dyDescent="0.35">
+      <c r="D31" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="E31" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="F31" s="11">
+        <v>2.1</v>
+      </c>
+    </row>
+    <row r="32" spans="4:6" x14ac:dyDescent="0.35">
+      <c r="D32" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E32" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="F32" s="11">
+        <v>13.26</v>
+      </c>
+    </row>
+    <row r="33" spans="4:6" x14ac:dyDescent="0.35">
+      <c r="D33" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="E33" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="F33" s="11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="4:6" x14ac:dyDescent="0.35">
+      <c r="D34" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="E34" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="F34" s="14">
+        <v>5.72</v>
+      </c>
+    </row>
+    <row r="35" spans="4:6" x14ac:dyDescent="0.35">
+      <c r="D35" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="E35" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="F35" s="15">
+        <v>5.69</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="6" tint="0.39997558519241921"/>
+  </sheetPr>
   <dimension ref="A1:AC27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="29.88671875" customWidth="1"/>
-    <col min="3" max="3" width="15.5546875" customWidth="1"/>
-    <col min="4" max="4" width="16.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="28" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.90625" customWidth="1"/>
+    <col min="3" max="3" width="15.54296875" customWidth="1"/>
+    <col min="4" max="4" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="28" width="14.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:29" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D1" s="6">
         <v>1</v>
       </c>
@@ -1625,7 +1741,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:29" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:29" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>53</v>
       </c>
@@ -1635,7 +1751,7 @@
       </c>
       <c r="AC2" s="5"/>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -1748,7 +1864,7 @@
       </c>
       <c r="AC3" s="3"/>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -1861,7 +1977,7 @@
       </c>
       <c r="AC4" s="3"/>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -1974,7 +2090,7 @@
       </c>
       <c r="AC5" s="3"/>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -2087,7 +2203,7 @@
       </c>
       <c r="AC6" s="3"/>
     </row>
-    <row r="7" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -2200,7 +2316,7 @@
       </c>
       <c r="AC7" s="3"/>
     </row>
-    <row r="8" spans="1:29" s="17" customFormat="1" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:29" s="17" customFormat="1" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="17" t="s">
         <v>68</v>
       </c>
@@ -2313,7 +2429,7 @@
       </c>
       <c r="AC8" s="18"/>
     </row>
-    <row r="9" spans="1:29" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:29" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
@@ -2341,14 +2457,14 @@
       <c r="AB9" s="3"/>
       <c r="AC9" s="3"/>
     </row>
-    <row r="10" spans="1:29" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:29" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>5</v>
       </c>
@@ -2433,7 +2549,7 @@
       </c>
       <c r="AC11" s="3"/>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -2542,7 +2658,7 @@
       </c>
       <c r="AC12" s="3"/>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -2651,7 +2767,7 @@
       </c>
       <c r="AC13" s="3"/>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -2760,7 +2876,7 @@
       </c>
       <c r="AC14" s="3"/>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -2869,7 +2985,7 @@
       </c>
       <c r="AC15" s="3"/>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.35">
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
@@ -2897,7 +3013,7 @@
       <c r="AB16" s="3"/>
       <c r="AC16" s="3"/>
     </row>
-    <row r="17" spans="1:29" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:29" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>13</v>
       </c>
@@ -2930,7 +3046,7 @@
       <c r="AB17" s="5"/>
       <c r="AC17" s="5"/>
     </row>
-    <row r="18" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>14</v>
       </c>
@@ -3039,7 +3155,7 @@
       </c>
       <c r="AC18" s="3"/>
     </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -3148,7 +3264,7 @@
       </c>
       <c r="AC19" s="3"/>
     </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>17</v>
       </c>
@@ -3257,7 +3373,7 @@
       </c>
       <c r="AC20" s="3"/>
     </row>
-    <row r="21" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -3366,7 +3482,7 @@
       </c>
       <c r="AC21" s="3"/>
     </row>
-    <row r="22" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -3475,7 +3591,7 @@
       </c>
       <c r="AC22" s="3"/>
     </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>20</v>
       </c>
@@ -3584,7 +3700,7 @@
       </c>
       <c r="AC23" s="3"/>
     </row>
-    <row r="24" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:29" x14ac:dyDescent="0.35">
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
@@ -3612,13 +3728,13 @@
       <c r="AB24" s="3"/>
       <c r="AC24" s="3"/>
     </row>
-    <row r="25" spans="1:29" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:29" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A25" s="2" t="s">
         <v>67</v>
       </c>
       <c r="AC25" s="5"/>
     </row>
-    <row r="26" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>54</v>
       </c>
@@ -3727,7 +3843,7 @@
         <v>7.8760683801125317E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:29" x14ac:dyDescent="0.35">
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
@@ -3759,7 +3875,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="6" tint="0.39997558519241921"/>
@@ -3770,47 +3886,47 @@
       <selection activeCell="AB5" sqref="AB5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="28" max="28" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="B1" s="22" t="s">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="B1" s="25" t="s">
         <v>74</v>
       </c>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
-      <c r="M1" s="22"/>
-      <c r="P1" s="23" t="s">
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
+      <c r="M1" s="25"/>
+      <c r="P1" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="Q1" s="23"/>
-      <c r="R1" s="23"/>
-      <c r="S1" s="23"/>
-      <c r="T1" s="23"/>
-      <c r="U1" s="23"/>
-      <c r="V1" s="23"/>
-      <c r="W1" s="23"/>
-      <c r="X1" s="23"/>
-      <c r="Y1" s="23"/>
-      <c r="Z1" s="23"/>
-      <c r="AA1" s="23"/>
-    </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="Q1" s="26"/>
+      <c r="R1" s="26"/>
+      <c r="S1" s="26"/>
+      <c r="T1" s="26"/>
+      <c r="U1" s="26"/>
+      <c r="V1" s="26"/>
+      <c r="W1" s="26"/>
+      <c r="X1" s="26"/>
+      <c r="Y1" s="26"/>
+      <c r="Z1" s="26"/>
+      <c r="AA1" s="26"/>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.35">
       <c r="B2" s="6" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:28" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>55</v>
       </c>
@@ -3893,7 +4009,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>1</v>
       </c>
@@ -4001,7 +4117,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>2</v>
       </c>
@@ -4105,7 +4221,7 @@
         <v>3.9451155333333374</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>3</v>
       </c>
@@ -4209,7 +4325,7 @@
         <v>30.917833333333331</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>4</v>
       </c>
@@ -4313,7 +4429,7 @@
         <v>34.86294886666667</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>5</v>
       </c>
@@ -4366,7 +4482,7 @@
         <v>20.611888888887904</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>6</v>
       </c>
@@ -4419,7 +4535,7 @@
         <v>18.035402777776795</v>
       </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>7</v>
       </c>
@@ -4472,7 +4588,7 @@
         <v>15.458916666665685</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>8</v>
       </c>
@@ -4525,7 +4641,7 @@
         <v>12.882430555554574</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>9</v>
       </c>
@@ -4578,7 +4694,7 @@
         <v>10.305944444443464</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>10</v>
       </c>
@@ -4631,7 +4747,7 @@
         <v>7.729458333332353</v>
       </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>11</v>
       </c>
@@ -4684,7 +4800,7 @@
         <v>5.1529722222212424</v>
       </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>12</v>
       </c>
@@ -4737,13 +4853,13 @@
         <v>2.5764861111101318</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B17" s="6" t="s">
         <v>56</v>
       </c>
       <c r="P17" s="6"/>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>1</v>
       </c>
@@ -4796,7 +4912,7 @@
         <v>0.32875962777776718</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>2</v>
       </c>
@@ -4849,7 +4965,7 @@
         <v>0.30136299212961909</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>3</v>
       </c>
@@ -4902,7 +5018,7 @@
         <v>0.27396635648147094</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>4</v>
       </c>
@@ -4955,7 +5071,7 @@
         <v>0.24656972083332285</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>5</v>
       </c>
@@ -5008,7 +5124,7 @@
         <v>0.2191730851851747</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>6</v>
       </c>
@@ -5061,7 +5177,7 @@
         <v>0.19177644953702658</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>7</v>
       </c>
@@ -5114,7 +5230,7 @@
         <v>0.16437981388887846</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>8</v>
       </c>
@@ -5167,7 +5283,7 @@
         <v>0.13698317824073031</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>9</v>
       </c>
@@ -5220,7 +5336,7 @@
         <v>0.10958654259258216</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>10</v>
       </c>
@@ -5273,7 +5389,7 @@
         <v>8.2189906944434024E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>11</v>
       </c>
@@ -5326,7 +5442,7 @@
         <v>5.4793271296285875E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>12</v>
       </c>
@@ -5379,7 +5495,7 @@
         <v>2.7396635648137733E-2</v>
       </c>
     </row>
-    <row r="31" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
         <v>57</v>
       </c>
@@ -5432,13 +5548,13 @@
         <v>2.13693758055543</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B33" s="6" t="s">
         <v>64</v>
       </c>
       <c r="P33" s="6"/>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>1</v>
       </c>
@@ -5491,7 +5607,7 @@
         <v>2.9052457388888779</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>2</v>
       </c>
@@ -5544,7 +5660,7 @@
         <v>2.8778491032407296</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>3</v>
       </c>
@@ -5597,7 +5713,7 @@
         <v>2.8504524675925813</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>4</v>
       </c>
@@ -5650,7 +5766,7 @@
         <v>2.8230558319444334</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>5</v>
       </c>
@@ -5703,7 +5819,7 @@
         <v>2.7956591962962851</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>6</v>
       </c>
@@ -5756,7 +5872,7 @@
         <v>2.7682625606481372</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>7</v>
       </c>
@@ -5809,7 +5925,7 @@
         <v>2.7408659249999889</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>8</v>
       </c>
@@ -5862,7 +5978,7 @@
         <v>2.7134692893518411</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>9</v>
       </c>
@@ -5915,7 +6031,7 @@
         <v>2.6860726537036927</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>10</v>
       </c>
@@ -5968,7 +6084,7 @@
         <v>2.6586760180555444</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>11</v>
       </c>
@@ -6021,7 +6137,7 @@
         <v>2.6312793824073966</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>12</v>
       </c>
@@ -6074,7 +6190,7 @@
         <v>2.6038827467592482</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.35">
       <c r="C47" s="8"/>
     </row>
   </sheetData>
@@ -6087,7 +6203,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="6" tint="0.39997558519241921"/>
@@ -6098,13 +6214,13 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="33.77734375" customWidth="1"/>
-    <col min="2" max="2" width="10.77734375" customWidth="1"/>
+    <col min="1" max="1" width="33.81640625" customWidth="1"/>
+    <col min="2" max="2" width="10.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:27" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:27" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
         <v>58</v>
       </c>
@@ -6184,7 +6300,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A3" s="6" t="s">
         <v>59</v>
       </c>
@@ -6292,7 +6408,7 @@
         <v>2.216605982300766</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
         <v>61</v>
       </c>
@@ -6400,7 +6516,7 @@
         <v>15.798787616666667</v>
       </c>
     </row>
-    <row r="5" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
         <v>62</v>
       </c>
@@ -6508,7 +6624,7 @@
         <v>3.9898907681413784</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A6" s="6"/>
       <c r="B6" s="6"/>
       <c r="C6" s="3"/>
@@ -6537,7 +6653,7 @@
       <c r="Z6" s="3"/>
       <c r="AA6" s="3"/>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A7" s="6" t="s">
         <v>63</v>
       </c>
@@ -6645,7 +6761,7 @@
         <v>18.015393598967432</v>
       </c>
     </row>
-    <row r="8" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:27" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>18</v>
       </c>

</xml_diff>